<commit_message>
admil track and card modification
</commit_message>
<xml_diff>
--- a/ACCOUNT/Account__12344.xlsx
+++ b/ACCOUNT/Account__12344.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,7 +561,7 @@
     <row r="9" ht="17.25" customHeight="1">
       <c r="A9" s="8" t="inlineStr">
         <is>
-          <t>BALANCE : 99874.0</t>
+          <t>BALANCE : 113.0</t>
         </is>
       </c>
     </row>
@@ -735,6 +735,168 @@
       </c>
       <c r="D19" t="n">
         <v>99874</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-10-21 18:54:38</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>109874</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:00:17</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>234</v>
+      </c>
+      <c r="D21" t="n">
+        <v>110108</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:01:33</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>110111</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:06:41</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
+        <v>110112</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:06:47</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>110113</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:36:06</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Withdraw</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D25" t="n">
+        <v>10113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:36:34</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Withdraw</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D26" t="n">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:54:59</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="D27" t="n">
+        <v>10000113</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-10-21 19:57:16</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Withdraw</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="D28" t="n">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
degine chande and fix tranjaction problam
</commit_message>
<xml_diff>
--- a/ACCOUNT/Account__12344.xlsx
+++ b/ACCOUNT/Account__12344.xlsx
@@ -16,13 +16,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -58,24 +64,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -449,7 +461,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,13 +469,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="9" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17.25" customHeight="1">
+    <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>BANK NAME : BRAINWARE BAKWAS BANK</t>
@@ -471,432 +483,484 @@
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>Account Holder</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>moumi day</t>
         </is>
       </c>
-      <c r="C2" s="7" t="n"/>
-      <c r="D2" s="7" t="n"/>
+      <c r="C2" s="5" t="n"/>
+      <c r="D2" s="5" t="n"/>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Account Number</t>
         </is>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>123444</v>
-      </c>
-      <c r="C3" s="7" t="n"/>
-      <c r="D3" s="7" t="n"/>
+      <c r="B3" s="5" t="n">
+        <v>12344</v>
+      </c>
+      <c r="C3" s="5" t="n"/>
+      <c r="D3" s="5" t="n"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Aadhar NO</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>123456</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="n"/>
-      <c r="D4" s="7" t="n"/>
+      <c r="B4" s="8" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C4" s="5" t="n"/>
+      <c r="D4" s="5" t="n"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Mail ID</t>
         </is>
       </c>
-      <c r="B5" s="6" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>moumiday91@gmail.com</t>
         </is>
       </c>
-      <c r="C5" s="7" t="n"/>
-      <c r="D5" s="7" t="n"/>
+      <c r="C5" s="5" t="n"/>
+      <c r="D5" s="5" t="n"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>DOB</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>29-08-2006</t>
         </is>
       </c>
-      <c r="C6" s="7" t="n"/>
-      <c r="D6" s="7" t="n"/>
+      <c r="C6" s="5" t="n"/>
+      <c r="D6" s="5" t="n"/>
     </row>
     <row r="7" ht="17.25" customHeight="1">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>UNP</t>
         </is>
       </c>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="7" t="n"/>
+      <c r="C7" s="5" t="n"/>
+      <c r="D7" s="5" t="n"/>
     </row>
     <row r="8" ht="17.25" customHeight="1">
-      <c r="A8" s="6" t="n"/>
-      <c r="B8" s="6" t="n"/>
-      <c r="C8" s="7" t="n"/>
-      <c r="D8" s="7" t="n"/>
-    </row>
-    <row r="9" ht="17.25" customHeight="1">
-      <c r="A9" s="8" t="inlineStr">
-        <is>
-          <t>BALANCE : 113.0</t>
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="8" t="n"/>
+      <c r="C8" s="5" t="n"/>
+      <c r="D8" s="5" t="n"/>
+    </row>
+    <row r="9" ht="18.75" customHeight="1">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>BALANCE : 400.0</t>
         </is>
       </c>
     </row>
     <row r="10" ht="17.25" customHeight="1">
-      <c r="A10" s="6" t="n"/>
-      <c r="B10" s="6" t="n"/>
-      <c r="C10" s="7" t="n"/>
-      <c r="D10" s="7" t="n"/>
+      <c r="A10" s="7" t="n"/>
+      <c r="B10" s="8" t="n"/>
+      <c r="C10" s="5" t="n"/>
+      <c r="D10" s="5" t="n"/>
     </row>
     <row r="11" ht="17.25" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="8" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr">
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="D11" s="7" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>New Balance</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="17.25" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
+    <row r="12" ht="18.75" customHeight="1">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:18:22</t>
         </is>
       </c>
-      <c r="B12" s="6" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C12" s="5" t="n">
+      <c r="B12" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="n">
         <v>1000</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="6" t="n">
         <v>2000</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+    <row r="13" ht="17.25" customHeight="1">
+      <c r="A13" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:19:49</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" s="5" t="n">
         <v>1800</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+    <row r="14" ht="17.25" customHeight="1">
+      <c r="A14" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:20:04</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" s="5" t="n">
         <v>1800</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" s="5" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+    <row r="15" ht="17.25" customHeight="1">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:20:49</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
+      <c r="B15" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="n">
         <v>100000</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" s="5" t="n">
         <v>100000</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="16" ht="17.25" customHeight="1">
+      <c r="A16" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:29:17</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" s="5" t="n">
         <v>99999</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+    <row r="17" ht="17.25" customHeight="1">
+      <c r="A17" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:29:20</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" s="5" t="n">
         <v>99998</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="18" ht="17.25" customHeight="1">
+      <c r="A18" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:29:23</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" s="5" t="n">
         <v>99997</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="19" ht="17.25" customHeight="1">
+      <c r="A19" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 16:29:29</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" s="5" t="n">
         <v>99874</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+    <row r="20" ht="17.25" customHeight="1">
+      <c r="A20" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 18:54:38</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" s="5" t="n">
         <v>109874</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="21" ht="17.25" customHeight="1">
+      <c r="A21" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:00:17</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
+      <c r="B21" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="n">
         <v>234</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21" s="5" t="n">
         <v>110108</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+    <row r="22" ht="17.25" customHeight="1">
+      <c r="A22" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:01:33</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
+      <c r="B22" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22" s="5" t="n">
         <v>110111</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="23" ht="17.25" customHeight="1">
+      <c r="A23" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:06:41</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23" s="5" t="n">
         <v>110112</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+    <row r="24" ht="17.25" customHeight="1">
+      <c r="A24" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:06:47</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
+      <c r="B24" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24" s="5" t="n">
         <v>110113</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="25" ht="17.25" customHeight="1">
+      <c r="A25" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:36:06</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" s="5" t="n">
         <v>100000</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25" s="5" t="n">
         <v>10113</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+    <row r="26" ht="17.25" customHeight="1">
+      <c r="A26" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:36:34</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" s="5" t="n">
         <v>10000</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26" s="5" t="n">
         <v>113</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="27" ht="17.25" customHeight="1">
+      <c r="A27" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:54:59</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Deposit</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="n">
         <v>10000000</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27" s="5" t="n">
         <v>10000113</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+    <row r="28" ht="17.25" customHeight="1">
+      <c r="A28" s="7" t="inlineStr">
         <is>
           <t>2025-10-21 19:57:16</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="8" t="inlineStr">
         <is>
           <t>Withdraw</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" s="5" t="n">
         <v>10000000</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28" s="5" t="n">
         <v>113</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-10-21 20:40:04</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>120</v>
+      </c>
+      <c r="D29" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-10-21 20:40:12</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>77</v>
+      </c>
+      <c r="D30" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-10-21 20:40:28</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>90</v>
+      </c>
+      <c r="D31" t="n">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pdf button and modify tranjaction show
</commit_message>
<xml_diff>
--- a/ACCOUNT/Account__12344.xlsx
+++ b/ACCOUNT/Account__12344.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -571,7 +571,7 @@
     <row r="9" ht="18.75" customHeight="1">
       <c r="A9" s="10" t="inlineStr">
         <is>
-          <t>BALANCE : 400.0</t>
+          <t>BALANCE : 10000524.0</t>
         </is>
       </c>
     </row>
@@ -961,6 +961,78 @@
       </c>
       <c r="D31" t="n">
         <v>400</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-10-21 20:45:54</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Withdraw</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="n">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-10-21 20:46:47</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>2</v>
+      </c>
+      <c r="D33" t="n">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-10-21 20:53:11</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>123</v>
+      </c>
+      <c r="D34" t="n">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-10-21 21:25:42</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Deposit</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="D35" t="n">
+        <v>10000524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>